<commit_message>
adding ex4 + test class to test times for matrixes
</commit_message>
<xml_diff>
--- a/Aula01.xlsx
+++ b/Aula01.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WorkspaceIntelliJSSD\TAED\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE2A21A8-6D6D-42BF-BB27-6EFB06E70902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE89D453-63B2-472D-BA9A-3420288311C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{F4E9959D-9745-4FC4-9FF1-6FDD6B7A1C2A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{F4E9959D-9745-4FC4-9FF1-6FDD6B7A1C2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Ex1" sheetId="1" r:id="rId1"/>
     <sheet name="Ex1 (2)" sheetId="3" r:id="rId2"/>
     <sheet name="Ex1 (3)" sheetId="5" r:id="rId3"/>
+    <sheet name="Ex1 (4)" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="5">
   <si>
     <t>N</t>
   </si>
@@ -50,6 +52,9 @@
   </si>
   <si>
     <t>x̄ Comparações</t>
+  </si>
+  <si>
+    <t>N * M</t>
   </si>
 </sst>
 </file>
@@ -99,15 +104,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -115,11 +126,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -132,11 +154,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="24">
     <dxf>
       <font>
         <b val="0"/>
@@ -190,6 +214,116 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -1629,34 +1763,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50</c:v>
+                  <c:v>3750</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100</c:v>
+                  <c:v>30000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>500</c:v>
+                  <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1000</c:v>
+                  <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>50000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>100000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>500000</c:v>
+                  <c:v>1000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1668,34 +1790,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.5</c:v>
+                  <c:v>4.0999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.34</c:v>
+                  <c:v>33.82</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.32</c:v>
+                  <c:v>179.84</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.46</c:v>
+                  <c:v>593.53899999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.32</c:v>
+                  <c:v>5630.1989999999996</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>56.58</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>102.599</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>459.09899999999999</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>754.88</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3183.68</c:v>
+                  <c:v>4229.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1704,6 +1814,495 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-7074-4901-B33F-E7532AD22FF6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="711240432"/>
+        <c:axId val="711237072"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="711240432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR"/>
+                  <a:t>número</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pt-BR" baseline="0"/>
+                  <a:t> de entradas (n)</a:t>
+                </a:r>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="711237072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="711237072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR"/>
+                  <a:t>x̄ Tempo (</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="el-GR"/>
+                  <a:t>μ</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pt-BR"/>
+                  <a:t>icro</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pt-BR" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pt-BR"/>
+                  <a:t>Ssegundos)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="711240432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0">
+                <a:latin typeface="+mj-lt"/>
+              </a:rPr>
+              <a:t>Tempo</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" baseline="0">
+                <a:latin typeface="+mj-lt"/>
+              </a:rPr>
+              <a:t> de execução em função do número de entrada</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1400" b="0">
+              <a:latin typeface="+mj-lt"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Tempo / N</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Ex1 (4)'!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Ex1 (4)'!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.34</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.52</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>54.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3341.56</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4263.9799999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>396516.84</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-148F-476E-B19A-5ED5C1A13681}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2139,6 +2738,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="241">
   <cs:axisTitle>
@@ -3180,6 +3819,526 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="241">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="241">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3787,16 +4946,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>586740</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>874608</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>148590</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>499534</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>148590</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3826,44 +4985,102 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>586740</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>148590</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>148590</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64768897-5730-406B-8997-E1624D5A1FD2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{99ADFC17-0B51-4E50-9E3A-442A272D0423}" name="Tabela1" displayName="Tabela1" ref="A1:D11" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{99ADFC17-0B51-4E50-9E3A-442A272D0423}" name="Tabela1" displayName="Tabela1" ref="A1:D11" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="A1:D11" xr:uid="{99ADFC17-0B51-4E50-9E3A-442A272D0423}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{F9862ECF-84F2-4CCD-8557-6C68FE5BA037}" name="N" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{47A90E9E-F011-4E3B-89C8-851D06BF2973}" name="x̄ Tempo (μS)" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{BD9712EA-934E-411A-B1B8-6E7FDBDB89F9}" name="x̄ Operações Aritiméticas" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{F29E9A37-650A-42C6-8EEF-963A0D68A312}" name="x̄ Comparações" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{F9862ECF-84F2-4CCD-8557-6C68FE5BA037}" name="N" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{47A90E9E-F011-4E3B-89C8-851D06BF2973}" name="x̄ Tempo (μS)" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{BD9712EA-934E-411A-B1B8-6E7FDBDB89F9}" name="x̄ Operações Aritiméticas" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{F29E9A37-650A-42C6-8EEF-963A0D68A312}" name="x̄ Comparações" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{70F34701-349A-4613-8C2F-434E03E9A3C5}" name="Tabela14" displayName="Tabela14" ref="A1:D11" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{70F34701-349A-4613-8C2F-434E03E9A3C5}" name="Tabela14" displayName="Tabela14" ref="A1:D11" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="A1:D11" xr:uid="{99ADFC17-0B51-4E50-9E3A-442A272D0423}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{A1D5FD59-8D59-4A61-98BB-A56EB7DCB1EA}" name="N" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{AABACD9E-DC37-451C-B877-64A57B1D31C5}" name="x̄ Tempo (μS)" dataDxfId="8">
+    <tableColumn id="1" xr3:uid="{A1D5FD59-8D59-4A61-98BB-A56EB7DCB1EA}" name="N" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{AABACD9E-DC37-451C-B877-64A57B1D31C5}" name="x̄ Tempo (μS)" dataDxfId="14">
       <calculatedColumnFormula>F2/$G$2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B1D4EF65-FF8C-4F00-B502-7C7806846983}" name="x̄ Operações Aritiméticas" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{E0D439F2-D115-4BD9-B737-E52C5C979396}" name="x̄ Comparações" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{B1D4EF65-FF8C-4F00-B502-7C7806846983}" name="x̄ Operações Aritiméticas" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{E0D439F2-D115-4BD9-B737-E52C5C979396}" name="x̄ Comparações" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F99BE0C2-A3D4-4EE9-AE8E-CEF2EDDBA763}" name="Tabela143" displayName="Tabela143" ref="A1:D11" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F99BE0C2-A3D4-4EE9-AE8E-CEF2EDDBA763}" name="Tabela143" displayName="Tabela143" ref="A1:D11" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A1:D11" xr:uid="{99ADFC17-0B51-4E50-9E3A-442A272D0423}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{B8462198-78EC-4165-8055-82A389D40410}" name="N" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{DBB55FE0-3A6B-4137-9FCE-DEEB41AB27F9}" name="x̄ Tempo (μS)" dataDxfId="2">
+    <tableColumn id="1" xr3:uid="{B8462198-78EC-4165-8055-82A389D40410}" name="N * M" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{DBB55FE0-3A6B-4137-9FCE-DEEB41AB27F9}" name="x̄ Tempo (μS)" dataDxfId="8">
       <calculatedColumnFormula>F2/$G$2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{A9A207B9-8151-4054-8581-6C1E99A8193B}" name="x̄ Operações Aritiméticas" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{0263E8F7-97D8-4E0B-98C3-C4338C794184}" name="x̄ Comparações" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{A9A207B9-8151-4054-8581-6C1E99A8193B}" name="x̄ Operações Aritiméticas" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{0263E8F7-97D8-4E0B-98C3-C4338C794184}" name="x̄ Comparações" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C9B3B8E9-7C6E-4DF8-8DF9-5055300A86F9}" name="Tabela145" displayName="Tabela145" ref="A1:D11" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D11" xr:uid="{99ADFC17-0B51-4E50-9E3A-442A272D0423}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{B9A2F950-2C9B-48E7-B1A0-CA6213626052}" name="N" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{DA531A9E-9079-4EBD-AFBB-5B48E8D20815}" name="x̄ Tempo (μS)" dataDxfId="2">
+      <calculatedColumnFormula>F2/$G$2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{D24A4035-75EE-41EB-8117-F4284B31E529}" name="x̄ Operações Aritiméticas" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{492784A3-DD7E-409A-8763-87F0C635C771}" name="x̄ Comparações" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4628,8 +5845,196 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E566EDF7-4850-499C-AA96-A5798C41A05F}">
   <dimension ref="A1:M11"/>
   <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="4" width="26.109375" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="9" max="9" width="13.5546875" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" customWidth="1"/>
+    <col min="11" max="11" width="14.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="42" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:13" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>100</v>
+      </c>
+      <c r="B2" s="3">
+        <f t="shared" ref="B2:B7" si="0">F2/$G$2</f>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C2" s="3">
+        <v>101</v>
+      </c>
+      <c r="D2" s="3">
+        <v>110</v>
+      </c>
+      <c r="F2">
+        <v>4100</v>
+      </c>
+      <c r="G2">
+        <v>1000</v>
+      </c>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>3750</v>
+      </c>
+      <c r="B3" s="3">
+        <f t="shared" si="0"/>
+        <v>33.82</v>
+      </c>
+      <c r="C3" s="3">
+        <v>3751</v>
+      </c>
+      <c r="D3" s="3">
+        <v>3800</v>
+      </c>
+      <c r="F3">
+        <v>33820</v>
+      </c>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>30000</v>
+      </c>
+      <c r="B4" s="3">
+        <f t="shared" si="0"/>
+        <v>179.84</v>
+      </c>
+      <c r="C4" s="3">
+        <v>30001</v>
+      </c>
+      <c r="D4" s="3">
+        <v>30100</v>
+      </c>
+      <c r="F4">
+        <v>179840</v>
+      </c>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>100000</v>
+      </c>
+      <c r="B5" s="3">
+        <f t="shared" si="0"/>
+        <v>593.53899999999999</v>
+      </c>
+      <c r="C5" s="3">
+        <v>100001</v>
+      </c>
+      <c r="D5" s="3">
+        <v>100500</v>
+      </c>
+      <c r="F5">
+        <v>593539</v>
+      </c>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>100000</v>
+      </c>
+      <c r="B6" s="3">
+        <f t="shared" si="0"/>
+        <v>5630.1989999999996</v>
+      </c>
+      <c r="C6" s="3">
+        <v>100001</v>
+      </c>
+      <c r="D6" s="3">
+        <v>200000</v>
+      </c>
+      <c r="F6">
+        <v>5630199</v>
+      </c>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="B7" s="3">
+        <f t="shared" si="0"/>
+        <v>4229.3</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1000001</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1001000</v>
+      </c>
+      <c r="F7">
+        <v>4229300</v>
+      </c>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="H8" s="1"/>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:13" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="H11" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B07D4CBF-4B1F-4FE3-9608-5D4FF067C65E}">
+  <dimension ref="A1:M11"/>
+  <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4662,16 +6067,16 @@
       </c>
       <c r="B2" s="3">
         <f>F2/$G$2</f>
-        <v>0.5</v>
+        <v>1.34</v>
       </c>
       <c r="C2" s="3">
-        <v>10</v>
+        <v>221</v>
       </c>
       <c r="D2" s="3">
-        <v>10</v>
-      </c>
-      <c r="F2">
-        <v>500</v>
+        <v>120</v>
+      </c>
+      <c r="F2" s="6">
+        <v>1340</v>
       </c>
       <c r="G2">
         <v>1000</v>
@@ -4683,17 +6088,17 @@
         <v>50</v>
       </c>
       <c r="B3" s="3">
-        <f t="shared" ref="B3:B11" si="0">F3/$G$2</f>
-        <v>1.34</v>
+        <f t="shared" ref="B3:B7" si="0">F3/$G$2</f>
+        <v>15.52</v>
       </c>
       <c r="C3" s="3">
-        <v>50</v>
+        <v>5101</v>
       </c>
       <c r="D3" s="3">
-        <v>50</v>
-      </c>
-      <c r="F3">
-        <v>1340</v>
+        <v>2600</v>
+      </c>
+      <c r="F3" s="7">
+        <v>15520</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -4703,16 +6108,16 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" si="0"/>
-        <v>1.32</v>
+        <v>54.2</v>
       </c>
       <c r="C4" s="3">
-        <v>100</v>
+        <v>20201</v>
       </c>
       <c r="D4" s="3">
-        <v>100</v>
-      </c>
-      <c r="F4">
-        <v>1320</v>
+        <v>10200</v>
+      </c>
+      <c r="F4" s="6">
+        <v>54200</v>
       </c>
       <c r="H4" s="1"/>
     </row>
@@ -4722,16 +6127,16 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" si="0"/>
-        <v>6.46</v>
+        <v>3341.56</v>
       </c>
       <c r="C5" s="3">
-        <v>500</v>
+        <v>501001</v>
       </c>
       <c r="D5" s="3">
-        <v>500</v>
-      </c>
-      <c r="F5">
-        <v>6460</v>
+        <v>251000</v>
+      </c>
+      <c r="F5" s="7">
+        <v>3341560</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -4741,16 +6146,16 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" si="0"/>
-        <v>11.32</v>
+        <v>4263.9799999999996</v>
       </c>
       <c r="C6" s="3">
-        <v>1000</v>
+        <v>2002001</v>
       </c>
       <c r="D6" s="3">
-        <v>1000</v>
-      </c>
-      <c r="F6">
-        <v>11320</v>
+        <v>1002000</v>
+      </c>
+      <c r="F6" s="6">
+        <v>4263980</v>
       </c>
       <c r="H6" s="1"/>
     </row>
@@ -4760,33 +6165,24 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" si="0"/>
-        <v>56.58</v>
+        <v>396516.84</v>
       </c>
       <c r="C7" s="3">
-        <v>5000</v>
+        <v>50010001</v>
       </c>
       <c r="D7" s="3">
-        <v>5000</v>
-      </c>
-      <c r="F7">
-        <v>56580</v>
+        <v>25010000</v>
+      </c>
+      <c r="F7" s="7">
+        <v>396516840</v>
       </c>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:13" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>10000</v>
-      </c>
-      <c r="B8" s="3">
-        <f t="shared" si="0"/>
-        <v>102.599</v>
-      </c>
-      <c r="C8" s="3">
-        <v>10000</v>
-      </c>
-      <c r="D8" s="3">
-        <v>10000</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
       <c r="F8">
         <v>102599</v>
       </c>
@@ -4794,57 +6190,30 @@
       <c r="M8" s="2"/>
     </row>
     <row r="9" spans="1:13" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>50000</v>
-      </c>
-      <c r="B9" s="3">
-        <f t="shared" si="0"/>
-        <v>459.09899999999999</v>
-      </c>
-      <c r="C9" s="3">
-        <v>50000</v>
-      </c>
-      <c r="D9" s="3">
-        <v>50000</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
       <c r="F9">
         <v>459099</v>
       </c>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:13" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <v>100000</v>
-      </c>
-      <c r="B10" s="3">
-        <f t="shared" si="0"/>
-        <v>754.88</v>
-      </c>
-      <c r="C10" s="3">
-        <v>100000</v>
-      </c>
-      <c r="D10" s="3">
-        <v>100000</v>
-      </c>
+      <c r="A10" s="1"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
       <c r="F10">
         <v>754880</v>
       </c>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:13" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>500000</v>
-      </c>
-      <c r="B11" s="3">
-        <f t="shared" si="0"/>
-        <v>3183.68</v>
-      </c>
-      <c r="C11" s="3">
-        <v>500000</v>
-      </c>
-      <c r="D11" s="3">
-        <v>500000</v>
-      </c>
+      <c r="A11" s="1"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
       <c r="F11">
         <v>3183680</v>
       </c>

</xml_diff>